<commit_message>
git commit -m 'Merge files git by error'
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1335 - 2HR, Jorge Armando Hernández_OC/Calidad/No_conformidades_P1335.xlsx
+++ b/Proyectos/2015/11/P1335 - 2HR, Jorge Armando Hernández_OC/Calidad/No_conformidades_P1335.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>REPORTE DE NO CONFORMIDADES P1339 - DA3 - CBANT, Héctor Antonio Núñez Ruiz_OC
 </t>
@@ -48,7 +48,7 @@
     <t>Oriana Osiris</t>
   </si>
   <si>
-    <t>En proceso</t>
+    <t>Cerrada</t>
   </si>
   <si>
     <t>No se requiere expresar en documento si no se presento algún cambio</t>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>No se comunico la creación de la linea base</t>
-  </si>
-  <si>
-    <t>Cerrada</t>
   </si>
   <si>
     <t>Se debe informar sobre la línea base mediante correo por cada proyecto entrante</t>
@@ -325,8 +322,8 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -514,10 +511,10 @@
         <v>42353</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,7 +522,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
@@ -540,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>